<commit_message>
Correction: Use acronym 2,4-DMA instead of 2,4-DME
</commit_message>
<xml_diff>
--- a/data/pesticides/2025-04-09_BDM_Results_Project79.xlsx
+++ b/data/pesticides/2025-04-09_BDM_Results_Project79.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bd379\xampp\htdocs\codeprojects\orei-analysis\data\pesticides\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bd379\xampp\htdocs\codeprojects\orei-organic-honey\data\pesticides\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A6C1E6-5CF5-489F-BD76-8257C5154FAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19ADCE03-5BFC-49C0-A1DC-91C958D9BBA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="0" windowWidth="21600" windowHeight="12336" activeTab="1" xr2:uid="{72D1E64B-17D5-45ED-8F25-CF6BE238CDDA}"/>
+    <workbookView xWindow="-28920" yWindow="-8130" windowWidth="29040" windowHeight="15720" xr2:uid="{72D1E64B-17D5-45ED-8F25-CF6BE238CDDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Wax" sheetId="1" r:id="rId1"/>
@@ -1924,7 +1924,7 @@
     <t>2,4-DMPF</t>
   </si>
   <si>
-    <t>2,4-DME</t>
+    <t>2,4-DMA</t>
   </si>
 </sst>
 </file>
@@ -2867,7 +2867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F405D6-B841-4034-8C7D-E78A0DB67A05}">
   <dimension ref="A1:DB84"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -26060,8 +26060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9DEE3D-ACFE-4831-849C-BD2CB626163C}">
   <dimension ref="B1:DB165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J86" sqref="J86"/>
+    <sheetView topLeftCell="A77" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L83" sqref="L83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>

</xml_diff>